<commit_message>
MS7 - FOX_PROC_GET_USER_PROFILING_DATA || Sp Fixation And Update Excel Sheat - DB Schema By Muhammad Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AbdulSattar\Fox\Latest Fox Works From 09-09-2020\Important files\Fox Procedures and Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammadsalman7\source\repos\FOXTEMp\FoxRehabilitationAPI\About Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="680">
   <si>
     <t>Table Names</t>
   </si>
@@ -2039,13 +2039,43 @@
   </si>
   <si>
     <t>PATIENT_STATEMENT_HISTORY</t>
+  </si>
+  <si>
+    <t>FOX_PROC_EXISTING_SURVEY_DETAIL</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_AUTOMATED_PERFORM_SURVEY_DETAILS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_PATIENT_SURVEY_DETAILS_SERVICE</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_PERFORM_SURVEY_PATIENT_DETAILS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_SMS_AND_EMAIL_DETAILS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_SURVEY_PATIENT_DETAILS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_INSERT_PATIENT_SURVEY_SERVICE_LOG</t>
+  </si>
+  <si>
+    <t>FOX_TBL_SURVEY_AUTOMATION_SERVICE_LOG</t>
+  </si>
+  <si>
+    <t>FOX_TBL_SURVEY_QUESTION</t>
+  </si>
+  <si>
+    <t>FOX_TBL_AUTOMATED_SURVEY_UNSUBSCRIPTION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2056,6 +2086,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2075,7 +2113,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2098,11 +2136,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2112,6 +2161,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2392,10 +2443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B211"/>
+  <dimension ref="A1:B214"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4092,6 +4143,30 @@
         <v>636</v>
       </c>
     </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>677</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>678</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>679</v>
+      </c>
+      <c r="B214" s="8" t="s">
+        <v>636</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:B211"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4101,10 +4176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A458"/>
+  <dimension ref="A1:A465"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6402,6 +6477,41 @@
         <v>668</v>
       </c>
     </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="7" t="s">
+        <v>676</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A458"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MS7 - Survey automation - DB Schema By Muhammad Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="681">
   <si>
     <t>Table Names</t>
   </si>
@@ -2069,13 +2069,16 @@
   </si>
   <si>
     <t>FOX_TBL_AUTOMATED_SURVEY_UNSUBSCRIPTION</t>
+  </si>
+  <si>
+    <t>InsertSource_AdditionalInfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2086,14 +2089,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2151,7 +2146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2161,7 +2156,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -4147,7 +4141,7 @@
       <c r="A212" t="s">
         <v>677</v>
       </c>
-      <c r="B212" s="8" t="s">
+      <c r="B212" s="7" t="s">
         <v>636</v>
       </c>
     </row>
@@ -4155,7 +4149,7 @@
       <c r="A213" t="s">
         <v>678</v>
       </c>
-      <c r="B213" s="8" t="s">
+      <c r="B213" s="7" t="s">
         <v>636</v>
       </c>
     </row>
@@ -4163,7 +4157,7 @@
       <c r="A214" t="s">
         <v>679</v>
       </c>
-      <c r="B214" s="8" t="s">
+      <c r="B214" s="7" t="s">
         <v>636</v>
       </c>
     </row>
@@ -4176,10 +4170,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A465"/>
+  <dimension ref="A1:A466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A449" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A468" sqref="A468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6508,8 +6502,13 @@
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="7" t="s">
+      <c r="A465" t="s">
         <v>676</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MS7 - DB Schema changes - Db Schema by Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammadsalman7\source\repos\FOXTEMp\FoxRehabilitationAPI\About Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammadsalman7\source\repos\FoxRehabilitationAPITest\FoxRehabilitationAPI\About Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="685">
   <si>
     <t>Table Names</t>
   </si>
@@ -2072,13 +2072,25 @@
   </si>
   <si>
     <t>InsertSource_AdditionalInfo</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_WORK_QUEUE_DETAILS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_WORK_QUEUE_FILE_ALL_DETAILS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_DELETE_ADMISSION_IMPORTANT_NOTES</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_NOTES_TYPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2089,6 +2101,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2146,7 +2165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2157,6 +2176,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4170,10 +4190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A466"/>
+  <dimension ref="A1:A470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A449" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A468" sqref="A468"/>
+    <sheetView tabSelected="1" topLeftCell="A451" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A470" sqref="A470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6511,6 +6531,26 @@
         <v>680</v>
       </c>
     </row>
+    <row r="467" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A467" s="8" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>684</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A458"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
About Project - API By Aftab khan
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammadsalman7\source\repos\FOXTEMp\FoxRehabilitationAPI\About Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aftabkhan\source\repos\API\SURVEY-API\FoxRehabilitationAPI\About Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="683">
   <si>
     <t>Table Names</t>
   </si>
@@ -2072,6 +2072,12 @@
   </si>
   <si>
     <t>InsertSource_AdditionalInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOX_PROC_GET_PATIENT_PENDING_BALANCE_NEW_LOGIC                          </t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_PENDING_HIGH_BALANCE_DETAILED_REPORT_NEW_LOGIC</t>
   </si>
 </sst>
 </file>
@@ -4170,10 +4176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A466"/>
+  <dimension ref="A1:A468"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A449" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A468" sqref="A468"/>
+      <selection activeCell="A473" sqref="A473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6511,6 +6517,16 @@
         <v>680</v>
       </c>
     </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>682</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A458"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MS7 - Set Table schema - Db Schema BY Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aftabkhan\source\repos\API\SURVEY-API\FoxRehabilitationAPI\About Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammadsalman7\source\repos\FoxRehabilitationAPITest\FoxRehabilitationAPI\About Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="684">
   <si>
     <t>Table Names</t>
   </si>
@@ -2078,6 +2078,9 @@
   </si>
   <si>
     <t>FOX_PROC_GET_PENDING_HIGH_BALANCE_DETAILED_REPORT_NEW_LOGIC</t>
+  </si>
+  <si>
+    <t>FOX_TBL_PATIENT_SURVEY_NOT_ANSWERED_REASON</t>
   </si>
 </sst>
 </file>
@@ -2443,10 +2446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B215"/>
   <sheetViews>
-    <sheetView topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="B217" sqref="B217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4167,6 +4170,14 @@
         <v>636</v>
       </c>
     </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>683</v>
+      </c>
+      <c r="B215" s="7" t="s">
+        <v>636</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:B211"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4178,8 +4189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A468"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A449" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A473" sqref="A473"/>
+    <sheetView topLeftCell="A449" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A469" sqref="A469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
MS7 - Add Table in Excel - DB Schema by Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="685">
   <si>
     <t>Table Names</t>
   </si>
@@ -2081,6 +2081,9 @@
   </si>
   <si>
     <t>FOX_TBL_PATIENT_SURVEY_NOT_ANSWERED_REASON</t>
+  </si>
+  <si>
+    <t>Fox_TBL_TASK_WORK_INTERFACE_MAPPING</t>
   </si>
 </sst>
 </file>
@@ -2446,10 +2449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B215"/>
+  <dimension ref="A1:B216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="B217" sqref="B217"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A220" sqref="A220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4175,6 +4178,14 @@
         <v>683</v>
       </c>
       <c r="B215" s="7" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>684</v>
+      </c>
+      <c r="B216" s="7" t="s">
         <v>636</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MS7 - Admission Notes Fixation - API By Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="686">
   <si>
     <t>Table Names</t>
   </si>
@@ -2084,6 +2084,9 @@
   </si>
   <si>
     <t>FOX_PROC_GET_NOTES_TYPE</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_ADMISSION_NOTES_DETAILS</t>
   </si>
 </sst>
 </file>
@@ -4190,10 +4193,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A470"/>
+  <dimension ref="A1:A471"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A451" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A470" sqref="A470"/>
+      <selection activeCell="A471" sqref="A471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6551,6 +6554,11 @@
         <v>684</v>
       </c>
     </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>685</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A458"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MS7 - Sprint 24 Scripts - Db Schema By Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammadsalman7\source\repos\FoxRehabilitationAPITest\FoxRehabilitationAPI\About Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammadsalman7\GIT\FoxRehabilitationAPI\FoxRehabilitationAPI\About Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="692">
   <si>
     <t>Table Names</t>
   </si>
@@ -2087,6 +2087,24 @@
   </si>
   <si>
     <t>FOX_PROC_GET_ADMISSION_NOTES_DETAILS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_EXTERNAL_USER_INFO</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_INSURANCE_DETAILS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_PSR_DETAILED_REPORT_COUNT</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_WORK_QUEUE_DETAIL</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_WORK_QUEUE_FILE_ALL_LIST</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_WORK_QUEUE_FILE_ALL_RECORD</t>
   </si>
 </sst>
 </file>
@@ -4193,10 +4211,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A471"/>
+  <dimension ref="A1:A477"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A451" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A471" sqref="A471"/>
+      <selection activeCell="A477" sqref="A477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6559,6 +6577,36 @@
         <v>685</v>
       </c>
     </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>691</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A458"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MS7 - FOX:8927 || Consent To Care , DB Schema - DB Schema By Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="707">
   <si>
     <t>Table Names</t>
   </si>
@@ -2105,6 +2105,51 @@
   </si>
   <si>
     <t>FOX_PROC_GET_WORK_QUEUE_FILE_ALL_RECORD</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_CASE_TRATEMENT_TEAM</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_CONSENT_TO_CARE_DETAILS_BY_CASE_ID</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_CONSENT_TO_CARE_DOCUMENTS_INFO</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_CONSENT_TO_CARE_INFO_BY_CASE_ID</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_CONSENT_TO_CARE_INFO_BY_CASE_ID_AND_SEND_TO</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_CONSENT_TO_CARE_INFO_BY_CONSENT_TO_CARE_ID</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_INSURANCE_DETAILS_FOR_CONSENT_TO_CARE</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_PATINET_CONTACT_DETAILS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_SERVICE_CONFIGURATION_CONSENT_TO_CARE</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_USER_ID_BY_PROVIDER_CODE</t>
+  </si>
+  <si>
+    <t>FOX_PROC_INSERT_CONSENT_TO_CARE_TASK</t>
+  </si>
+  <si>
+    <t>FOX_PROC_UPDATE_TASK_LOG</t>
+  </si>
+  <si>
+    <t>FOX_TBL_CONSENT_TO_CARE</t>
+  </si>
+  <si>
+    <t>FOX_TBL_CONSENT_TO_CARE_DOCUMENTS</t>
+  </si>
+  <si>
+    <t>FOX_TBL_CONSENT_TO_CARE_STATUS</t>
   </si>
 </sst>
 </file>
@@ -2478,10 +2523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B217"/>
   <sheetViews>
-    <sheetView topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4202,6 +4247,21 @@
         <v>636</v>
       </c>
     </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>706</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:B211"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4211,10 +4271,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A477"/>
+  <dimension ref="A1:A489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A477" sqref="A477"/>
+    <sheetView topLeftCell="A469" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A489" sqref="A489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6607,6 +6667,66 @@
         <v>691</v>
       </c>
     </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>703</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A458"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MS7 - FOX:8927 || Add Dev script & expiry Service scripts  - DB Schema By Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="710">
   <si>
     <t>Table Names</t>
   </si>
@@ -2150,6 +2150,15 @@
   </si>
   <si>
     <t>FOX_TBL_CONSENT_TO_CARE_STATUS</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_CONSENT_TO_CARE_FOR_EXPIRY</t>
+  </si>
+  <si>
+    <t>FOX_PROC_GET_CONSENT_STATUS_ID_BY_NAME</t>
+  </si>
+  <si>
+    <t>FOX_PROC_EXPIRE_CONSENT_TO_CARE_LINK</t>
   </si>
 </sst>
 </file>
@@ -2525,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="A217" sqref="A217"/>
+    <sheetView topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="A234" sqref="A234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4271,10 +4280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A489"/>
+  <dimension ref="A1:A492"/>
   <sheetViews>
-    <sheetView topLeftCell="A469" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A489" sqref="A489"/>
+    <sheetView tabSelected="1" topLeftCell="A469" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A496" sqref="A496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6727,6 +6736,21 @@
         <v>703</v>
       </c>
     </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>709</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A458"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MS7 - Kanban borad - Release  ABC 26 || Stored Procedure - DB Schema By Salman
</commit_message>
<xml_diff>
--- a/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
+++ b/FoxRehabilitationAPI/About Project/FoxPortalTablesProcedures.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="711">
   <si>
     <t>Table Names</t>
   </si>
@@ -2159,6 +2159,9 @@
   </si>
   <si>
     <t>FOX_PROC_EXPIRE_CONSENT_TO_CARE_LINK</t>
+  </si>
+  <si>
+    <t>FOX_PROC_INSERT_SINGLE_WORK_ORDER_HISTORY</t>
   </si>
 </sst>
 </file>
@@ -4280,10 +4283,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A492"/>
+  <dimension ref="A1:A493"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A469" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A496" sqref="A496"/>
+      <selection activeCell="A493" sqref="A493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6751,6 +6754,11 @@
         <v>709</v>
       </c>
     </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>710</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A458"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>